<commit_message>
DCP -7594 -Schedule rating, DCP-7666 - Advanced Risk Control code check in
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="123">
   <si>
     <t>testname</t>
   </si>
@@ -183,12 +183,6 @@
     <t>guidelinedeductible</t>
   </si>
   <si>
-    <t>selecteddeductible</t>
-  </si>
-  <si>
-    <t>quoteprmium</t>
-  </si>
-  <si>
     <t>priorclaimhistorystatus</t>
   </si>
   <si>
@@ -207,12 +201,6 @@
     <t>$500,000</t>
   </si>
   <si>
-    <t>finalpremium</t>
-  </si>
-  <si>
-    <t>option</t>
-  </si>
-  <si>
     <t>one</t>
   </si>
   <si>
@@ -319,6 +307,93 @@
   </si>
   <si>
     <t>test0716</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>FinancialCondition_value</t>
+  </si>
+  <si>
+    <t>FinancialCondition_comment</t>
+  </si>
+  <si>
+    <t>MaturityOfBusiness_comment</t>
+  </si>
+  <si>
+    <t>MaturityOfBusiness_value</t>
+  </si>
+  <si>
+    <t>VolumeOfInformationStored_value</t>
+  </si>
+  <si>
+    <t>VolumeOfInformationStored_comment</t>
+  </si>
+  <si>
+    <t>TerritoryofOperations_comment</t>
+  </si>
+  <si>
+    <t>TerritoryofOperations_value</t>
+  </si>
+  <si>
+    <t>Natureofcontent_value</t>
+  </si>
+  <si>
+    <t>Natureofcontent_comment</t>
+  </si>
+  <si>
+    <t>NatureOfPaymentCardProcessingExposure_value</t>
+  </si>
+  <si>
+    <t>NatureOfPaymentCardProcessingExposure_comment</t>
+  </si>
+  <si>
+    <t>NatureOfReputationalRiskExposure_value</t>
+  </si>
+  <si>
+    <t>NatureOfReputationalRiskExposure_comment</t>
+  </si>
+  <si>
+    <t>PrivacyandSecurityControls_value</t>
+  </si>
+  <si>
+    <t>PrivacyandSecurityControls_comment</t>
+  </si>
+  <si>
+    <t>ParticipationInRiskControlProgram_value</t>
+  </si>
+  <si>
+    <t>ParticipationInRiskControlProgram_comment</t>
+  </si>
+  <si>
+    <t>ScheduleRatingFactor</t>
+  </si>
+  <si>
+    <t>QualityOfManagement_value</t>
+  </si>
+  <si>
+    <t>QualityOfManagement_comment</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>limitanddeductibleoption</t>
+  </si>
+  <si>
+    <t>ransomwarecoinsurance</t>
+  </si>
+  <si>
+    <t>ransomwaresublimitliability</t>
+  </si>
+  <si>
+    <t>standardpremium</t>
+  </si>
+  <si>
+    <t>advancedriskcontrolcomment</t>
+  </si>
+  <si>
+    <t>advanced risk control test</t>
   </si>
 </sst>
 </file>
@@ -371,7 +446,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -394,12 +469,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -410,6 +496,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -719,7 +809,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>2</v>
@@ -727,10 +817,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>41</v>
@@ -744,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:CA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
+      <selection activeCell="CA2" sqref="CA2:CA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,10 +872,15 @@
     <col min="31" max="31" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="54" width="21.42578125" customWidth="1"/>
+    <col min="34" max="46" width="21.42578125" customWidth="1"/>
+    <col min="47" max="47" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="28" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="25.28515625" customWidth="1"/>
+    <col min="56" max="56" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,16 +927,16 @@
         <v>21</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>47</v>
@@ -862,19 +957,19 @@
         <v>27</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>43</v>
@@ -895,61 +990,130 @@
         <v>42</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AU1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="BE1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="BG1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="BH1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="BL1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="BM1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="BN1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="BO1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="BP1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="BQ1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="BR1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BY1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>60</v>
+      <c r="BZ1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CA1" s="12" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -957,13 +1121,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -981,7 +1145,7 @@
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>31</v>
@@ -990,7 +1154,7 @@
         <v>33</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>32</v>
@@ -1002,13 +1166,13 @@
         <v>34</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>35</v>
@@ -1020,28 +1184,28 @@
         <v>9</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AC2" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="AD2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>14</v>
@@ -1050,16 +1214,16 @@
         <v>40</v>
       </c>
       <c r="AH2" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AI2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK2" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK2" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="AL2" s="7" t="s">
         <v>2</v>
@@ -1077,57 +1241,132 @@
         <v>41</v>
       </c>
       <c r="AQ2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="AR2" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="AS2" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AT2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AV2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AX2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AY2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AZ2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="BA2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB2" s="7" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="BA2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BE2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BH2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BI2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BJ2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BK2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BL2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BN2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BO2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BQ2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="BS2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="BX2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="BZ2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="CA2" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -1145,7 +1384,7 @@
         <v>30</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>31</v>
@@ -1154,7 +1393,7 @@
         <v>33</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>32</v>
@@ -1166,13 +1405,13 @@
         <v>34</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>35</v>
@@ -1184,28 +1423,28 @@
         <v>9</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AB3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="AD3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF3" s="3" t="s">
         <v>14</v>
@@ -1214,16 +1453,16 @@
         <v>40</v>
       </c>
       <c r="AH3" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AI3" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ3" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK3" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AL3" s="7" t="s">
         <v>2</v>
@@ -1241,40 +1480,115 @@
         <v>41</v>
       </c>
       <c r="AQ3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR3" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="AR3" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="AS3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AT3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AV3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AX3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AY3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AZ3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="BA3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB3" s="7" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AZ3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BE3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BH3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BI3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BJ3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BK3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BL3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BN3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BO3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BQ3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="BS3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="BT3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="BU3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="BV3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="BX3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="BZ3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="CA3" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>